<commit_message>
trying url for imports
</commit_message>
<xml_diff>
--- a/terms/pelvisTerms.xlsx
+++ b/terms/pelvisTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308386F0-AD3A-064C-A16F-5DB9131CD192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23813DBD-8609-B448-BF3F-2825976F61EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16620" activeTab="2" xr2:uid="{B87B9758-12F3-EB43-B7F0-7CE57CABE0EE}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16620" activeTab="1" xr2:uid="{B87B9758-12F3-EB43-B7F0-7CE57CABE0EE}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -256,6 +256,30 @@
   </si>
   <si>
     <t>distal-most acetabular part of hip bone</t>
+  </si>
+  <si>
+    <t>This includes the three bones of the pelvis: the pubis, ischium, and ilium</t>
+  </si>
+  <si>
+    <t>pubic symphsis</t>
+  </si>
+  <si>
+    <t>ilium shaft</t>
+  </si>
+  <si>
+    <t>obtruartor foramen</t>
+  </si>
+  <si>
+    <t>tubera coxarum</t>
+  </si>
+  <si>
+    <t>tubera ischiadica</t>
+  </si>
+  <si>
+    <t>medial-lateral</t>
+  </si>
+  <si>
+    <t>circumfernce and ('inheres in' some 'shaft of ilium')</t>
   </si>
 </sst>
 </file>
@@ -632,7 +656,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,6 +780,9 @@
       <c r="F9" t="s">
         <v>34</v>
       </c>
+      <c r="I9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
@@ -814,15 +841,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7929AA-F3E1-154B-A335-23682B090A81}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,7 +858,7 @@
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -844,7 +872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -854,8 +882,11 @@
       <c r="C2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -866,53 +897,79 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
         <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -920,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB60FD1-5962-E64C-A0AF-EDCC1C415E7C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -975,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D975CF9-06D0-2D4C-8B77-2F5F54813A7F}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,6 +1087,26 @@
         <v>28</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>